<commit_message>
Added symbiont composition of each sample, dominant symbiont by depth with all data grouped together and broken down by genus
</commit_message>
<xml_diff>
--- a/Data/Sample_data/Ex_Sample_Data.xlsx
+++ b/Data/Sample_data/Ex_Sample_Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="194">
   <si>
     <t>sample_id</t>
   </si>
@@ -344,9 +344,6 @@
   </si>
   <si>
     <t>EX0062</t>
-  </si>
-  <si>
-    <t>psuedodiploria</t>
   </si>
   <si>
     <t>EX0063</t>
@@ -2721,7 +2718,7 @@
         <v>100</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>33</v>
@@ -2732,7 +2729,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B72" s="2">
         <v>43548.0</v>
@@ -2761,7 +2758,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B73" s="2">
         <v>43548.0</v>
@@ -2790,7 +2787,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B74" s="2">
         <v>43548.0</v>
@@ -2819,7 +2816,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B75" s="2">
         <v>43548.0</v>
@@ -2848,7 +2845,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B76" s="2">
         <v>43550.0</v>
@@ -2857,13 +2854,13 @@
         <v>12</v>
       </c>
       <c r="D76" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>19</v>
@@ -2877,7 +2874,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B77" s="2">
         <v>43550.0</v>
@@ -2886,13 +2883,13 @@
         <v>12</v>
       </c>
       <c r="D77" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="F77" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>16</v>
@@ -2906,7 +2903,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B78" s="2">
         <v>43550.0</v>
@@ -2915,13 +2912,13 @@
         <v>12</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="F78" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>28</v>
@@ -2935,7 +2932,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B79" s="2">
         <v>43550.0</v>
@@ -2944,13 +2941,13 @@
         <v>12</v>
       </c>
       <c r="D79" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="F79" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>16</v>
@@ -2962,12 +2959,12 @@
         <v>15.1</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B80" s="2">
         <v>43550.0</v>
@@ -2976,13 +2973,13 @@
         <v>12</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>19</v>
@@ -2996,7 +2993,7 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B81" s="2">
         <v>43550.0</v>
@@ -3005,13 +3002,13 @@
         <v>12</v>
       </c>
       <c r="D81" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>16</v>
@@ -3023,12 +3020,12 @@
         <v>14.6</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B82" s="2">
         <v>43550.0</v>
@@ -3037,13 +3034,13 @@
         <v>12</v>
       </c>
       <c r="D82" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>32</v>
@@ -3057,7 +3054,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B83" s="2">
         <v>43550.0</v>
@@ -3066,13 +3063,13 @@
         <v>12</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="F83" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>16</v>
@@ -3086,7 +3083,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B84" s="2">
         <v>43551.0</v>
@@ -3095,13 +3092,13 @@
         <v>12</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>16</v>
@@ -3115,7 +3112,7 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B85" s="2">
         <v>43551.0</v>
@@ -3124,13 +3121,13 @@
         <v>12</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="F85" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>19</v>
@@ -3144,7 +3141,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B86" s="2">
         <v>43551.0</v>
@@ -3153,13 +3150,13 @@
         <v>12</v>
       </c>
       <c r="D86" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>19</v>
@@ -3173,7 +3170,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B87" s="2">
         <v>43551.0</v>
@@ -3182,13 +3179,13 @@
         <v>12</v>
       </c>
       <c r="D87" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>16</v>
@@ -3202,7 +3199,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B88" s="2">
         <v>43551.0</v>
@@ -3211,13 +3208,13 @@
         <v>12</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>19</v>
@@ -3231,7 +3228,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B89" s="2">
         <v>43551.0</v>
@@ -3240,13 +3237,13 @@
         <v>12</v>
       </c>
       <c r="D89" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="F89" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>16</v>
@@ -3260,7 +3257,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B90" s="2">
         <v>43553.0</v>
@@ -3269,13 +3266,13 @@
         <v>12</v>
       </c>
       <c r="D90" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>28</v>
@@ -3289,7 +3286,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B91" s="2">
         <v>43553.0</v>
@@ -3298,13 +3295,13 @@
         <v>12</v>
       </c>
       <c r="D91" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>32</v>
@@ -3318,7 +3315,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B92" s="2">
         <v>43553.0</v>
@@ -3327,13 +3324,13 @@
         <v>12</v>
       </c>
       <c r="D92" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="F92" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>19</v>
@@ -3347,7 +3344,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B93" s="2">
         <v>43553.0</v>
@@ -3356,13 +3353,13 @@
         <v>12</v>
       </c>
       <c r="D93" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="F93" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>16</v>
@@ -3376,7 +3373,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B94" s="2">
         <v>43553.0</v>
@@ -3385,13 +3382,13 @@
         <v>12</v>
       </c>
       <c r="D94" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="F94" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>16</v>
@@ -3405,7 +3402,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B95" s="2">
         <v>43553.0</v>
@@ -3414,13 +3411,13 @@
         <v>12</v>
       </c>
       <c r="D95" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="F95" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>19</v>
@@ -3434,7 +3431,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B96" s="2">
         <v>43553.0</v>
@@ -3443,13 +3440,13 @@
         <v>12</v>
       </c>
       <c r="D96" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>16</v>
@@ -3463,7 +3460,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B97" s="2">
         <v>43553.0</v>
@@ -3472,13 +3469,13 @@
         <v>12</v>
       </c>
       <c r="D97" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>19</v>
@@ -3492,7 +3489,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B98" s="2">
         <v>43549.0</v>
@@ -3501,13 +3498,13 @@
         <v>12</v>
       </c>
       <c r="D98" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E98" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="F98" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>19</v>
@@ -3521,7 +3518,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B99" s="2">
         <v>43549.0</v>
@@ -3530,13 +3527,13 @@
         <v>12</v>
       </c>
       <c r="D99" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="F99" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>28</v>
@@ -3550,7 +3547,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B100" s="2">
         <v>43549.0</v>
@@ -3559,13 +3556,13 @@
         <v>12</v>
       </c>
       <c r="D100" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E100" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="F100" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>19</v>
@@ -3579,7 +3576,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B101" s="2">
         <v>43549.0</v>
@@ -3588,13 +3585,13 @@
         <v>12</v>
       </c>
       <c r="D101" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E101" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="F101" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>28</v>
@@ -3608,7 +3605,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B102" s="2">
         <v>43549.0</v>
@@ -3617,13 +3614,13 @@
         <v>12</v>
       </c>
       <c r="D102" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="F102" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>32</v>
@@ -3637,7 +3634,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B103" s="2">
         <v>43549.0</v>
@@ -3646,13 +3643,13 @@
         <v>12</v>
       </c>
       <c r="D103" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="F103" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>16</v>
@@ -3666,7 +3663,7 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B104" s="2">
         <v>43549.0</v>
@@ -3675,13 +3672,13 @@
         <v>12</v>
       </c>
       <c r="D104" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E104" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="F104" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>16</v>
@@ -3695,7 +3692,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B105" s="2">
         <v>43549.0</v>
@@ -3704,13 +3701,13 @@
         <v>12</v>
       </c>
       <c r="D105" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="F105" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>32</v>
@@ -3724,7 +3721,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B106" s="2">
         <v>43549.0</v>
@@ -3733,13 +3730,13 @@
         <v>12</v>
       </c>
       <c r="D106" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E106" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="F106" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>28</v>
@@ -3753,7 +3750,7 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B107" s="2">
         <v>43549.0</v>
@@ -3762,13 +3759,13 @@
         <v>12</v>
       </c>
       <c r="D107" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E107" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="F107" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>19</v>
@@ -3782,7 +3779,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B108" s="2">
         <v>43549.0</v>
@@ -3791,13 +3788,13 @@
         <v>12</v>
       </c>
       <c r="D108" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E108" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="F108" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>19</v>
@@ -3811,7 +3808,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B109" s="2">
         <v>43549.0</v>
@@ -3820,13 +3817,13 @@
         <v>12</v>
       </c>
       <c r="D109" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="F109" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>16</v>
@@ -3840,7 +3837,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B110" s="2">
         <v>43549.0</v>
@@ -3849,13 +3846,13 @@
         <v>12</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="F110" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>32</v>
@@ -3869,7 +3866,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B111" s="2">
         <v>43549.0</v>
@@ -3878,13 +3875,13 @@
         <v>12</v>
       </c>
       <c r="D111" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E111" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="F111" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>28</v>
@@ -3898,7 +3895,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B112" s="2">
         <v>43549.0</v>
@@ -3907,13 +3904,13 @@
         <v>12</v>
       </c>
       <c r="D112" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E112" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E112" s="1" t="s">
+      <c r="F112" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>19</v>
@@ -3927,7 +3924,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B113" s="2">
         <v>43549.0</v>
@@ -3936,13 +3933,13 @@
         <v>12</v>
       </c>
       <c r="D113" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E113" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="F113" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>32</v>
@@ -3956,7 +3953,7 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B114" s="2">
         <v>43549.0</v>
@@ -3965,13 +3962,13 @@
         <v>12</v>
       </c>
       <c r="D114" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E114" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E114" s="1" t="s">
+      <c r="F114" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>16</v>
@@ -3985,7 +3982,7 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B115" s="2">
         <v>43549.0</v>
@@ -3994,13 +3991,13 @@
         <v>12</v>
       </c>
       <c r="D115" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E115" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="F115" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>28</v>
@@ -4014,7 +4011,7 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B116" s="2">
         <v>43549.0</v>
@@ -4023,13 +4020,13 @@
         <v>12</v>
       </c>
       <c r="D116" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="F116" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>32</v>
@@ -4043,7 +4040,7 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B117" s="2">
         <v>43555.0</v>
@@ -4052,13 +4049,13 @@
         <v>12</v>
       </c>
       <c r="D117" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E117" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E117" s="1" t="s">
+      <c r="F117" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>32</v>
@@ -4069,7 +4066,7 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B118" s="2">
         <v>43555.0</v>
@@ -4078,13 +4075,13 @@
         <v>12</v>
       </c>
       <c r="D118" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="F118" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>16</v>
@@ -4095,7 +4092,7 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B119" s="2">
         <v>43555.0</v>
@@ -4104,13 +4101,13 @@
         <v>12</v>
       </c>
       <c r="D119" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E119" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>19</v>
@@ -4121,7 +4118,7 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B120" s="2">
         <v>43555.0</v>
@@ -4130,13 +4127,13 @@
         <v>12</v>
       </c>
       <c r="D120" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="F120" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>28</v>
@@ -4147,7 +4144,7 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B121" s="2">
         <v>43555.0</v>
@@ -4156,15 +4153,15 @@
         <v>12</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B122" s="2">
         <v>43555.0</v>
@@ -4173,13 +4170,13 @@
         <v>12</v>
       </c>
       <c r="D122" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="F122" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>19</v>
@@ -4188,12 +4185,12 @@
         <v>20</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B123" s="2">
         <v>43555.0</v>
@@ -4202,13 +4199,13 @@
         <v>12</v>
       </c>
       <c r="D123" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E123" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="F123" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>19</v>
@@ -4222,7 +4219,7 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B124" s="2">
         <v>43555.0</v>
@@ -4231,13 +4228,13 @@
         <v>12</v>
       </c>
       <c r="D124" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E124" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="F124" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>19</v>
@@ -4249,12 +4246,12 @@
         <v>3.6</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B125" s="2">
         <v>43555.0</v>
@@ -4263,13 +4260,13 @@
         <v>12</v>
       </c>
       <c r="D125" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E125" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E125" s="1" t="s">
+      <c r="F125" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>16</v>
@@ -4283,7 +4280,7 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B126" s="2">
         <v>43555.0</v>
@@ -4292,13 +4289,13 @@
         <v>12</v>
       </c>
       <c r="D126" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E126" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E126" s="1" t="s">
+      <c r="F126" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>16</v>
@@ -4312,7 +4309,7 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B127" s="2">
         <v>43555.0</v>
@@ -4321,13 +4318,13 @@
         <v>12</v>
       </c>
       <c r="D127" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E127" s="1" t="s">
+      <c r="F127" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>19</v>
@@ -4341,7 +4338,7 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B128" s="2">
         <v>43555.0</v>
@@ -4350,13 +4347,13 @@
         <v>12</v>
       </c>
       <c r="D128" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="F128" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>16</v>
@@ -4370,7 +4367,7 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B129" s="2">
         <v>43555.0</v>
@@ -4379,13 +4376,13 @@
         <v>12</v>
       </c>
       <c r="D129" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E129" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E129" s="1" t="s">
+      <c r="F129" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>16</v>
@@ -4397,12 +4394,12 @@
         <v>3.6</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B130" s="2">
         <v>43555.0</v>
@@ -4411,13 +4408,13 @@
         <v>12</v>
       </c>
       <c r="D130" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E130" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E130" s="1" t="s">
+      <c r="F130" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>16</v>
@@ -4431,7 +4428,7 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B131" s="2">
         <v>43555.0</v>
@@ -4440,13 +4437,13 @@
         <v>12</v>
       </c>
       <c r="D131" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E131" s="1" t="s">
+      <c r="F131" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>19</v>
@@ -4460,7 +4457,7 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B132" s="2">
         <v>43555.0</v>
@@ -4469,13 +4466,13 @@
         <v>12</v>
       </c>
       <c r="D132" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E132" s="1" t="s">
+      <c r="F132" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>19</v>
@@ -4489,7 +4486,7 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B133" s="2">
         <v>43555.0</v>
@@ -4498,13 +4495,13 @@
         <v>12</v>
       </c>
       <c r="D133" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E133" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E133" s="1" t="s">
+      <c r="F133" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>16</v>
@@ -4518,7 +4515,7 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B134" s="2">
         <v>43553.0</v>
@@ -4527,12 +4524,12 @@
         <v>12</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B135" s="2">
         <v>43553.0</v>
@@ -4541,7 +4538,7 @@
         <v>12</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>